<commit_message>
Aggiornamento stato task Burndown chart
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\PycharmProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DAE834-C016-4CD7-AF81-8868D92A26E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B0E419-1770-4D22-AB50-8A1458D3DA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>Santonicola Federico</t>
   </si>
   <si>
-    <t>Non iniziata</t>
-  </si>
-  <si>
     <t>US #2</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>US #7</t>
+  </si>
+  <si>
+    <t>Completata</t>
   </si>
 </sst>
 </file>
@@ -296,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -337,9 +337,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1945,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E092E5-C70C-4A02-95A3-9D8F5F48E490}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+    <sheetView zoomScale="73" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2078,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F59B876-E793-45F0-95C7-4E253C5C7DF4}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2131,12 +2128,12 @@
         <v>18</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="10">
         <v>2</v>
@@ -2147,67 +2144,67 @@
     </row>
     <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="10">
         <v>3</v>
@@ -2218,22 +2215,22 @@
     </row>
     <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="10">
         <v>3</v>
@@ -2244,52 +2241,52 @@
     </row>
     <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="10">
         <v>3</v>
@@ -2300,52 +2297,52 @@
     </row>
     <row r="16" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="10">
         <v>5</v>
@@ -2356,52 +2353,52 @@
     </row>
     <row r="20" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="10">
         <v>5</v>
@@ -2412,32 +2409,32 @@
     </row>
     <row r="24" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="D24" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento gestione click con tasto sinistro del mouse e burndown chart e review report
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\PycharmProjects\Progetto-SAD\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B0E419-1770-4D22-AB50-8A1458D3DA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F101B03A-8C53-49E6-9B39-8E435A6AAB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,13 +566,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,7 +661,7 @@
                   <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,13 +729,13 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E092E5-C70C-4A02-95A3-9D8F5F48E490}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2005,7 +2005,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <f xml:space="preserve"> D2 - B3</f>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="E3" s="2">
         <f xml:space="preserve"> E2 - C3</f>
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -2024,7 +2024,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D5" si="1" xml:space="preserve"> D3 - B4</f>
@@ -2032,7 +2032,7 @@
       </c>
       <c r="E4" s="2">
         <f t="shared" ref="E4:E5" si="2" xml:space="preserve"> E3 - C4</f>
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -2040,18 +2040,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -2075,7 +2075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F59B876-E793-45F0-95C7-4E253C5C7DF4}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="39" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="39" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornamento Stato dei task assegnati nel burndownChart (Sprint2)
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\IdeaProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F5027A-1D1C-4064-BAAA-ADCDD44F3620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5432DF9C-F6E0-408B-B90A-5A7DE5D90E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
   <si>
     <t>Sprint</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>TSK28: Voce "Taglia" menu contestuale forme</t>
-  </si>
-  <si>
-    <t>Non Iniziata</t>
   </si>
   <si>
     <t>US #16</t>
@@ -426,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -497,9 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2126,15 +2120,15 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
@@ -2177,7 +2171,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
@@ -2196,7 +2190,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2215,7 +2209,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2234,7 +2228,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2259,16 +2253,16 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="43.1796875" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" customWidth="1"/>
-    <col min="5" max="5" width="41.1796875" customWidth="1"/>
+    <col min="3" max="3" width="43.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" customWidth="1"/>
+    <col min="5" max="5" width="41.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2285,7 +2279,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2296,7 +2290,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="76.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -2311,7 +2305,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2322,7 +2316,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2337,7 +2331,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -2352,7 +2346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
@@ -2367,7 +2361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -2393,7 +2387,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
@@ -2408,7 +2402,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -2419,7 +2413,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2434,7 +2428,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2449,7 +2443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
@@ -2464,7 +2458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -2475,7 +2469,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
@@ -2490,7 +2484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>45</v>
       </c>
@@ -2505,7 +2499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>47</v>
       </c>
@@ -2520,7 +2514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -2531,7 +2525,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
@@ -2546,7 +2540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -2561,7 +2555,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>54</v>
       </c>
@@ -2576,7 +2570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -2587,7 +2581,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -2602,7 +2596,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="59.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="59.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>59</v>
       </c>
@@ -2630,20 +2624,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707AD77F-AD1F-4B96-8DA9-A040FF438B35}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.453125" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="77.54296875" customWidth="1"/>
-    <col min="4" max="4" width="33.1796875" customWidth="1"/>
-    <col min="5" max="5" width="37.453125" customWidth="1"/>
+    <col min="3" max="3" width="77.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2660,7 +2654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -2671,7 +2665,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>62</v>
       </c>
@@ -2686,7 +2680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -2697,7 +2691,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="48.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>64</v>
       </c>
@@ -2712,7 +2706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>77</v>
       </c>
@@ -2727,7 +2721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -2738,7 +2732,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>67</v>
       </c>
@@ -2753,7 +2747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>69</v>
       </c>
@@ -2764,7 +2758,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>70</v>
       </c>
@@ -2779,7 +2773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>71</v>
       </c>
@@ -2790,7 +2784,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>72</v>
       </c>
@@ -2805,7 +2799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>74</v>
       </c>
@@ -2816,7 +2810,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -2825,28 +2819,28 @@
         <v>76</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>83</v>
@@ -2855,7 +2849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>85</v>
       </c>
@@ -2866,22 +2860,22 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>84</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>86</v>
       </c>
@@ -2890,13 +2884,13 @@
         <v>87</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>88</v>
       </c>
@@ -2907,7 +2901,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>90</v>
       </c>
@@ -2916,15 +2910,15 @@
         <v>89</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="B22" s="10">
         <v>3</v>
@@ -2933,25 +2927,25 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:5" ht="59.75" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="E23" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:5" ht="59.7" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2962,20 +2956,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3129,6 +3123,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3140,14 +3142,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aggiustati e aggiornati per lo Sprint 2 il Burndown chart, lo Sprint Planning. Aggiunta del class diagram e del Review Report
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\IdeaProjects\Progetto-SAD\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\PycharmProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5432DF9C-F6E0-408B-B90A-5A7DE5D90E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C921D9-ED9B-4F1E-AAB1-D44EB13B71CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -681,7 +681,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,7 +821,7 @@
                   <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>103</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2116,19 +2116,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E092E5-C70C-4A02-95A3-9D8F5F48E490}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="98" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2209,26 +2209,26 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2253,16 +2253,16 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" customWidth="1"/>
-    <col min="5" max="5" width="41.21875" customWidth="1"/>
+    <col min="3" max="3" width="43.1796875" customWidth="1"/>
+    <col min="4" max="4" width="25.81640625" customWidth="1"/>
+    <col min="5" max="5" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2290,7 +2290,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="76.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>29</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -2413,7 +2413,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -2469,7 +2469,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>45</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>47</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -2525,7 +2525,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>54</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="59.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="59.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>59</v>
       </c>
@@ -2624,20 +2624,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707AD77F-AD1F-4B96-8DA9-A040FF438B35}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="77.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="77.54296875" customWidth="1"/>
+    <col min="4" max="4" width="33.1796875" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>62</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="48.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>64</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>77</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -2732,7 +2732,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>67</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>69</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>70</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>71</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>72</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>74</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
         <v>99</v>
       </c>
@@ -2834,7 +2834,7 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
         <v>97</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>85</v>
       </c>
@@ -2860,7 +2860,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>95</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>86</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>88</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>90</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>91</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>93</v>
       </c>
@@ -2942,10 +2942,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:5" ht="59.7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:5" ht="59.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2956,20 +2956,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3123,14 +3123,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3142,6 +3134,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
cambiati i task 30 e 31 della tabella Task Sprint 3, con le rispettive descrizioni
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\IdeaProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD5FCB3A-2BDF-45D5-85CA-DF3F793F53FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9216EBA-1568-4C95-942B-7F6FBCFB1D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
@@ -350,12 +350,6 @@
     <t>Non Iniziata</t>
   </si>
   <si>
-    <t>TSK31: Implementazione comandi eliminazione, ridimensiona, cambio colore e trascinamento</t>
-  </si>
-  <si>
-    <t>Implementare i comandi: DeleteCommand, ResizeCommand, ChangeColorCommand e DragCommand</t>
-  </si>
-  <si>
     <t>Effettuare il refactoring del controller affinchè utilizzi la logica dei Command</t>
   </si>
   <si>
@@ -450,23 +444,29 @@
 Modificare il ViewController sostituendo i cast espliciti da ShapeInterface con l’utilizzo di questo nuovo metodo.</t>
   </si>
   <si>
-    <t>TSK30: Implementazione comandi inserimento, taglia e incolla</t>
+    <t>Treglia Martina Rosaria</t>
+  </si>
+  <si>
+    <t>Aggiungere 4 radio button alla barra degli strumenti che al clic permettano di visualizzare con uno zoom differente lo spazio di lavoro, nei 4 livelli di zoom previsti</t>
+  </si>
+  <si>
+    <t>Masturzo Vincenzo Pietro Pio</t>
+  </si>
+  <si>
+    <t>Aggiungere alla barra degli strumenti un toggle button che quando selezionato permetta di attivare la visualizzazione di una griglia</t>
+  </si>
+  <si>
+    <t>TSK30: Implementazione comandi inserimento e trascinamento</t>
+  </si>
+  <si>
+    <t>TSK31: Implementazione comandi eliminazione, ridimensiona, cambio colore</t>
+  </si>
+  <si>
+    <t>Implementare i comandi: DeleteCommand, ResizeCommand, ChangeColorCommand</t>
   </si>
   <si>
     <t>Creare l’interfaccia Command.
-Successivamente implementare i comandi: InsertCommand, CutCommand, PasteCommand</t>
-  </si>
-  <si>
-    <t>Treglia Martina Rosaria</t>
-  </si>
-  <si>
-    <t>Aggiungere 4 radio button alla barra degli strumenti che al clic permettano di visualizzare con uno zoom differente lo spazio di lavoro, nei 4 livelli di zoom previsti</t>
-  </si>
-  <si>
-    <t>Masturzo Vincenzo Pietro Pio</t>
-  </si>
-  <si>
-    <t>Aggiungere alla barra degli strumenti un toggle button che quando selezionato permetta di attivare la visualizzazione di una griglia</t>
+Successivamente implementare i comandi: InsertCommand  e DragCommand</t>
   </si>
 </sst>
 </file>
@@ -1891,10 +1891,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C04064D0-0483-4F2B-8D80-6D3C94DE3902}" name="Tabella1" displayName="Tabella1" ref="A1:E5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:E5" xr:uid="{C04064D0-0483-4F2B-8D80-6D3C94DE3902}"/>
@@ -3116,7 +3112,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3158,11 +3154,11 @@
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
@@ -3173,11 +3169,11 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>85</v>
@@ -3188,11 +3184,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -3203,11 +3199,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>85</v>
@@ -3218,11 +3214,11 @@
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>18</v>
@@ -3233,7 +3229,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" s="10">
         <v>3</v>
@@ -3244,11 +3240,11 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>85</v>
@@ -3259,11 +3255,11 @@
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>18</v>
@@ -3274,7 +3270,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="10">
         <v>3</v>
@@ -3285,11 +3281,11 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>85</v>
@@ -3300,11 +3296,11 @@
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>18</v>
@@ -3315,7 +3311,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="10">
         <v>5</v>
@@ -3326,14 +3322,14 @@
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>101</v>
@@ -3341,7 +3337,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B16" s="10">
         <v>3</v>
@@ -3352,14 +3348,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>101</v>
@@ -3367,7 +3363,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B18" s="10">
         <v>2</v>
@@ -3378,14 +3374,14 @@
     </row>
     <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>101</v>
@@ -3393,7 +3389,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B20" s="28">
         <v>2</v>
@@ -3404,14 +3400,14 @@
     </row>
     <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>101</v>
@@ -3419,7 +3415,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" s="10">
         <v>3</v>
@@ -3430,14 +3426,14 @@
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>101</v>
@@ -3454,14 +3450,14 @@
     </row>
     <row r="25" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>101</v>
@@ -3479,15 +3475,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006D06A881EF84BF4D9C2E0A241D74C9AB" ma:contentTypeVersion="5" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="6ad53b5fb9ed4d9ca0953b41cd1c771f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cad3c75a-58d7-40e3-abd0-865ba3ea7957" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cacddd16a8291ce2bddd10790055ff38" ns3:_="">
     <xsd:import namespace="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
@@ -3637,6 +3624,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3646,14 +3642,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A080C301-2896-455C-B03E-90A728C8991F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3667,6 +3655,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aggiornate le task del burndown chart. Aggiunta la classe di test per il comando InsertCommand
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\IdeaProjects\Progetto-SAD\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\Progetti Java\Progetto_SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9216EBA-1568-4C95-942B-7F6FBCFB1D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F354891-A8FF-4EE8-9634-E38C8ADF8F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -456,17 +456,18 @@
     <t>Aggiungere alla barra degli strumenti un toggle button che quando selezionato permetta di attivare la visualizzazione di una griglia</t>
   </si>
   <si>
-    <t>TSK30: Implementazione comandi inserimento e trascinamento</t>
-  </si>
-  <si>
-    <t>TSK31: Implementazione comandi eliminazione, ridimensiona, cambio colore</t>
-  </si>
-  <si>
-    <t>Implementare i comandi: DeleteCommand, ResizeCommand, ChangeColorCommand</t>
-  </si>
-  <si>
-    <t>Creare l’interfaccia Command.
-Successivamente implementare i comandi: InsertCommand  e DragCommand</t>
+    <t>TSK30: Implementazione comandi inserimento, eliminazione e trascinamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creare l’interfaccia Command.
+Successivamente implementare i comandi: InsertCommand, DeleteCommand  e DragCommand
+</t>
+  </si>
+  <si>
+    <t>TSK31: Implementazione comandi ridimensiona, cambio colore bordi e cambio colore riempimento</t>
+  </si>
+  <si>
+    <t>Implementare i comandi: ResizeCommand, ChangeStrokeColorCommand e ChangeFillColorCommand</t>
   </si>
 </sst>
 </file>
@@ -3112,12 +3113,12 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="78.33203125" customWidth="1"/>
+    <col min="1" max="1" width="84.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="87.21875" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" customWidth="1"/>
@@ -3152,13 +3153,13 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
@@ -3169,11 +3170,11 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>85</v>
@@ -3475,6 +3476,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006D06A881EF84BF4D9C2E0A241D74C9AB" ma:contentTypeVersion="5" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="6ad53b5fb9ed4d9ca0953b41cd1c771f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cad3c75a-58d7-40e3-abd0-865ba3ea7957" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cacddd16a8291ce2bddd10790055ff38" ns3:_="">
     <xsd:import namespace="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
@@ -3624,24 +3642,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A080C301-2896-455C-B03E-90A728C8991F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3657,28 +3682,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornamento stato dei task della Sprint3
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\Progetti Java\Progetto_SAD\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\IdeaProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F354891-A8FF-4EE8-9634-E38C8ADF8F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540D5E28-60A3-4C9D-80D5-8830345F72BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
   <si>
     <t>Sprint</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>US #17</t>
-  </si>
-  <si>
-    <t>Non Iniziata</t>
   </si>
   <si>
     <t>Effettuare il refactoring del controller affinchè utilizzi la logica dei Command</t>
@@ -474,7 +471,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +504,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -550,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -631,6 +636,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2778,7 +2784,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3110,10 +3116,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2B26B3-2611-4BA2-A2BF-A1C920DED04D}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3155,82 +3161,82 @@
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="10">
         <v>3</v>
@@ -3241,37 +3247,37 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="10">
         <v>3</v>
@@ -3282,37 +3288,37 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="10">
         <v>5</v>
@@ -3323,22 +3329,22 @@
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="10">
         <v>3</v>
@@ -3349,22 +3355,22 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="10">
         <v>2</v>
@@ -3375,22 +3381,22 @@
     </row>
     <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="28">
         <v>2</v>
@@ -3401,22 +3407,22 @@
     </row>
     <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="10">
         <v>3</v>
@@ -3427,17 +3433,17 @@
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3451,20 +3457,23 @@
     </row>
     <row r="25" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>135</v>
+        <v>18</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="30"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3476,23 +3485,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006D06A881EF84BF4D9C2E0A241D74C9AB" ma:contentTypeVersion="5" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="6ad53b5fb9ed4d9ca0953b41cd1c771f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cad3c75a-58d7-40e3-abd0-865ba3ea7957" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cacddd16a8291ce2bddd10790055ff38" ns3:_="">
     <xsd:import namespace="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
@@ -3642,31 +3634,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cad3c75a-58d7-40e3-abd0-865ba3ea7957" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A080C301-2896-455C-B03E-90A728C8991F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3682,4 +3667,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornamento Burndown chart per lo Sprint 3
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Desktop\Progetti Java\Progetto_SAD\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\PycharmProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F354891-A8FF-4EE8-9634-E38C8ADF8F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2041CA37-2B8D-473B-BCA5-BFF34A0CCB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
   <si>
     <t>Sprint</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>US #17</t>
-  </si>
-  <si>
-    <t>Non Iniziata</t>
   </si>
   <si>
     <t>Effettuare il refactoring del controller affinchè utilizzi la logica dei Command</t>
@@ -474,7 +471,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +504,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -550,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -631,6 +636,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -871,7 +877,7 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1034,7 +1040,7 @@
                   <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2269,19 +2275,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E092E5-C70C-4A02-95A3-9D8F5F48E490}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="98" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2298,7 +2304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
@@ -2378,10 +2384,10 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2402,20 +2408,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F59B876-E793-45F0-95C7-4E253C5C7DF4}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScaleSheetLayoutView="37" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="68" zoomScaleNormal="68" zoomScaleSheetLayoutView="37" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="43.36328125" customWidth="1"/>
+    <col min="4" max="4" width="25.6328125" customWidth="1"/>
+    <col min="5" max="5" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2443,7 +2449,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="91.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -2458,7 +2464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2469,7 +2475,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>29</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -2540,7 +2546,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -2566,7 +2572,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2596,7 +2602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
@@ -2611,7 +2617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -2622,7 +2628,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="45.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>45</v>
       </c>
@@ -2652,7 +2658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>47</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -2678,7 +2684,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>50</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
@@ -2708,7 +2714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>54</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -2734,7 +2740,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="59.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="59.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>59</v>
       </c>
@@ -2777,20 +2783,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707AD77F-AD1F-4B96-8DA9-A040FF438B35}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A12" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="37" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="77.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="77.54296875" customWidth="1"/>
+    <col min="4" max="4" width="33.36328125" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
@@ -2818,7 +2824,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>62</v>
       </c>
@@ -2833,7 +2839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>65</v>
       </c>
@@ -2844,7 +2850,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="48.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>66</v>
       </c>
@@ -2859,7 +2865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>72</v>
       </c>
@@ -2885,7 +2891,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="29.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="29.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>73</v>
       </c>
@@ -2900,7 +2906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2911,7 +2917,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>77</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>79</v>
       </c>
@@ -2937,7 +2943,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>80</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>82</v>
       </c>
@@ -2963,7 +2969,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>83</v>
       </c>
@@ -2978,7 +2984,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
         <v>86</v>
       </c>
@@ -2987,7 +2993,7 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
         <v>87</v>
       </c>
@@ -3002,7 +3008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>89</v>
       </c>
@@ -3013,7 +3019,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>90</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>92</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>94</v>
       </c>
@@ -3054,7 +3060,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>95</v>
       </c>
@@ -3069,7 +3075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>97</v>
       </c>
@@ -3080,12 +3086,12 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="70.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>98</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -3095,10 +3101,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="31.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:5" ht="58.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:5" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:5" ht="59.7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="30"/>
+    </row>
+    <row r="27" spans="1:5" ht="32.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:5" ht="59.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3110,22 +3118,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2B26B3-2611-4BA2-A2BF-A1C920DED04D}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="84.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="87.21875" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="87.1796875" customWidth="1"/>
+    <col min="4" max="4" width="33.36328125" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3142,7 +3150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -3153,84 +3161,84 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="10">
         <v>3</v>
@@ -3239,39 +3247,39 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="10">
         <v>3</v>
@@ -3280,39 +3288,39 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="10">
         <v>5</v>
@@ -3321,24 +3329,24 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="10">
         <v>3</v>
@@ -3346,25 +3354,26 @@
       <c r="C16" s="29"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="10">
         <v>2</v>
@@ -3373,24 +3382,24 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="28">
         <v>2</v>
@@ -3399,24 +3408,24 @@
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="10">
         <v>3</v>
@@ -3425,22 +3434,22 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>86</v>
       </c>
@@ -3449,22 +3458,22 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>18</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3484,15 +3493,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006D06A881EF84BF4D9C2E0A241D74C9AB" ma:contentTypeVersion="5" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="6ad53b5fb9ed4d9ca0953b41cd1c771f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cad3c75a-58d7-40e3-abd0-865ba3ea7957" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cacddd16a8291ce2bddd10790055ff38" ns3:_="">
     <xsd:import namespace="cad3c75a-58d7-40e3-abd0-865ba3ea7957"/>
@@ -3642,6 +3642,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{717C791E-FCB3-40AD-88FF-A49361D61F2C}">
   <ds:schemaRefs>
@@ -3659,14 +3668,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A080C301-2896-455C-B03E-90A728C8991F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3682,4 +3683,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC5A00A-4000-42AF-9964-66AE6D943A28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornamento Burndown chart, Product backlog e Review Report dello Srint 3, relativo alla task 40.
</commit_message>
<xml_diff>
--- a/docs/Burndown chart.xlsx
+++ b/docs/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attil\PycharmProjects\Progetto-SAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2041CA37-2B8D-473B-BCA5-BFF34A0CCB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0614EF-BFD3-43DF-953D-A691F05C8A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{EB4EC49D-06D4-4331-8995-0B2882866B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="141">
   <si>
     <t>Sprint</t>
   </si>
@@ -384,9 +384,6 @@
   </si>
   <si>
     <t>Aggiungere al menu contestuale delle forme la voce "Porta dietro", che, quando selezionata permetta di fornire la priorità visiva minima alla forma selezionata</t>
-  </si>
-  <si>
-    <t>Gestire l’operazione del panning dello spazio di lavoro e la sua conseguente espansione</t>
   </si>
   <si>
     <t>Implementare la disattivazione della griglia quando il toggle button della barra degli strumenti viene deselezionato</t>
@@ -465,6 +462,12 @@
   </si>
   <si>
     <t>Implementare i comandi: ResizeCommand, ChangeStrokeColorCommand e ChangeFillColorCommand</t>
+  </si>
+  <si>
+    <t>Non completata</t>
+  </si>
+  <si>
+    <t>Gestire il panning dello spazio di lavoro e l'espansione automatica quando una forma viene trascinata oltre i bordi visibili.</t>
   </si>
 </sst>
 </file>
@@ -877,7 +880,7 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,7 +1043,7 @@
                   <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2275,8 +2278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E092E5-C70C-4A02-95A3-9D8F5F48E490}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="98" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2376,7 +2379,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="2">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
@@ -2384,7 +2387,7 @@
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -3120,8 +3123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2B26B3-2611-4BA2-A2BF-A1C920DED04D}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="37" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3163,11 +3166,11 @@
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
@@ -3178,11 +3181,11 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>85</v>
@@ -3193,11 +3196,11 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -3208,7 +3211,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="8" t="s">
@@ -3223,7 +3226,7 @@
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
@@ -3249,7 +3252,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="12" t="s">
@@ -3264,7 +3267,7 @@
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="12" t="s">
@@ -3290,7 +3293,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="12" t="s">
@@ -3305,7 +3308,7 @@
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="12" t="s">
@@ -3331,14 +3334,14 @@
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>19</v>
@@ -3356,19 +3359,19 @@
       <c r="E16" s="4"/>
       <c r="H16" s="30"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="12" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>19</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -3384,14 +3387,14 @@
     </row>
     <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>19</v>
@@ -3410,14 +3413,14 @@
     </row>
     <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>19</v>
@@ -3436,14 +3439,14 @@
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>19</v>
@@ -3460,11 +3463,11 @@
     </row>
     <row r="25" spans="1:5" ht="58.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>18</v>

</xml_diff>